<commit_message>
create sum of all sales more than 00 using SUMIF function
</commit_message>
<xml_diff>
--- a/working_with_conditions.xlsx
+++ b/working_with_conditions.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HP\Desktop\Projects\Data_Analysis_Portfolio\working_with_conditions\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A03F9E55-EDDF-49EB-B95C-C03A3D9FCB76}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87FB4ABF-8D05-4AD6-8B90-4C982C953BBB}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7545" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="38">
   <si>
     <t>Name</t>
   </si>
@@ -132,6 +132,9 @@
   <si>
     <t>No. of Saleperson</t>
   </si>
+  <si>
+    <t>Sales over $500</t>
+  </si>
 </sst>
 </file>
 
@@ -140,7 +143,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -158,6 +161,14 @@
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -181,7 +192,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -194,6 +205,7 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -412,7 +424,7 @@
   <dimension ref="A1:J1000"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="F5" workbookViewId="0">
-      <selection activeCell="I17" sqref="I17"/>
+      <selection activeCell="I8" sqref="I8:I10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.25" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -424,9 +436,9 @@
     <col min="5" max="5" width="13.625" customWidth="1"/>
     <col min="6" max="6" width="16" customWidth="1"/>
     <col min="7" max="7" width="11.125" customWidth="1"/>
-    <col min="8" max="8" width="11.125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="8.625" customWidth="1"/>
-    <col min="10" max="25" width="10.5" customWidth="1"/>
+    <col min="8" max="8" width="8.625" customWidth="1"/>
+    <col min="9" max="9" width="15.25" bestFit="1" customWidth="1"/>
+    <col min="10" max="24" width="10.5" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -571,12 +583,6 @@
       <c r="G6" s="4">
         <v>119.89100000000002</v>
       </c>
-      <c r="H6" t="s">
-        <v>1</v>
-      </c>
-      <c r="I6" t="s">
-        <v>8</v>
-      </c>
     </row>
     <row r="7" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
@@ -601,13 +607,6 @@
       <c r="G7" s="4">
         <v>16.836000000000002</v>
       </c>
-      <c r="H7" t="s">
-        <v>36</v>
-      </c>
-      <c r="I7">
-        <f>COUNTIF(B2:B21, "NY")</f>
-        <v>6</v>
-      </c>
     </row>
     <row r="8" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
@@ -632,6 +631,12 @@
       <c r="G8" s="4">
         <v>166.661</v>
       </c>
+      <c r="I8" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="J8" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="9" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
@@ -656,6 +661,13 @@
       <c r="G9" s="4">
         <v>91.028999999999996</v>
       </c>
+      <c r="I9" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="J9">
+        <f>COUNTIF(B2:B21, "NY")</f>
+        <v>6</v>
+      </c>
     </row>
     <row r="10" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
@@ -680,6 +692,13 @@
       <c r="G10" s="4">
         <v>63.169000000000011</v>
       </c>
+      <c r="I10" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="J10">
+        <f>SUMIF(D2:D21, "&gt;500")</f>
+        <v>19007.61</v>
+      </c>
     </row>
     <row r="11" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
@@ -776,7 +795,7 @@
       <c r="G14" s="4">
         <v>33.258000000000003</v>
       </c>
-      <c r="I14" s="5" t="s">
+      <c r="H14" s="5" t="s">
         <v>28</v>
       </c>
     </row>
@@ -827,7 +846,7 @@
       <c r="G16" s="4">
         <v>38.949000000000005</v>
       </c>
-      <c r="J16" s="3"/>
+      <c r="I16" s="3"/>
     </row>
     <row r="17" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
@@ -4867,6 +4886,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
-  <pageSetup orientation="landscape"/>
+  <pageSetup orientation="landscape" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Sum only the sales from New York using SUMIF function
</commit_message>
<xml_diff>
--- a/working_with_conditions.xlsx
+++ b/working_with_conditions.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HP\Desktop\Projects\Data_Analysis_Portfolio\working_with_conditions\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87FB4ABF-8D05-4AD6-8B90-4C982C953BBB}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3AC52E57-E80E-48D7-8D3B-7DB5A0B0E7E7}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7545" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="39">
   <si>
     <t>Name</t>
   </si>
@@ -134,6 +134,9 @@
   </si>
   <si>
     <t>Sales over $500</t>
+  </si>
+  <si>
+    <t>NY sales</t>
   </si>
 </sst>
 </file>
@@ -423,8 +426,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F5" workbookViewId="0">
-      <selection activeCell="I8" sqref="I8:I10"/>
+    <sheetView tabSelected="1" topLeftCell="H4" workbookViewId="0">
+      <selection activeCell="J19" sqref="J19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.25" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -723,6 +726,13 @@
       <c r="G11" s="4">
         <v>76.532000000000011</v>
       </c>
+      <c r="I11" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="J11">
+        <f>SUMIF(B2:B21, "NY", D2:D21)</f>
+        <v>5417.3000000000011</v>
+      </c>
     </row>
     <row r="12" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">

</xml_diff>

<commit_message>
calculate average sales per salesperson in New York
</commit_message>
<xml_diff>
--- a/working_with_conditions.xlsx
+++ b/working_with_conditions.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HP\Desktop\Projects\Data_Analysis_Portfolio\working_with_conditions\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3AC52E57-E80E-48D7-8D3B-7DB5A0B0E7E7}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89563E2E-C4DB-4162-B572-2E78957914EF}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7545" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="40">
   <si>
     <t>Name</t>
   </si>
@@ -137,6 +137,9 @@
   </si>
   <si>
     <t>NY sales</t>
+  </si>
+  <si>
+    <t>Average sales NY</t>
   </si>
 </sst>
 </file>
@@ -426,8 +429,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H4" workbookViewId="0">
-      <selection activeCell="J19" sqref="J19"/>
+    <sheetView tabSelected="1" topLeftCell="H3" workbookViewId="0">
+      <selection activeCell="K17" sqref="K17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.25" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -757,6 +760,13 @@
       <c r="G12" s="4">
         <v>133.66800000000001</v>
       </c>
+      <c r="I12" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="J12">
+        <f>AVERAGEIF(B2:B21, "NY",D2:D21)</f>
+        <v>902.88333333333355</v>
+      </c>
     </row>
     <row r="13" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">

</xml_diff>

<commit_message>
find max sales from any salesperson in NY
</commit_message>
<xml_diff>
--- a/working_with_conditions.xlsx
+++ b/working_with_conditions.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HP\Desktop\Projects\Data_Analysis_Portfolio\working_with_conditions\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89563E2E-C4DB-4162-B572-2E78957914EF}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4984338-7221-4A06-9D16-D83D65777A10}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7545" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="41">
   <si>
     <t>Name</t>
   </si>
@@ -139,7 +139,10 @@
     <t>NY sales</t>
   </si>
   <si>
-    <t>Average sales NY</t>
+    <t>Average sales (NY)</t>
+  </si>
+  <si>
+    <t>Max sales (NY)</t>
   </si>
 </sst>
 </file>
@@ -429,8 +432,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H3" workbookViewId="0">
-      <selection activeCell="K17" sqref="K17"/>
+    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
+      <selection activeCell="K13" sqref="K13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.25" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -791,6 +794,13 @@
       <c r="G13" s="4">
         <v>70.915999999999997</v>
       </c>
+      <c r="I13" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="J13">
+        <f>_xlfn.MAXIFS(D2:D21,B2:B21, "NY")</f>
+        <v>1666.61</v>
+      </c>
     </row>
     <row r="14" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">

</xml_diff>

<commit_message>
find maximum sales in New York where the Max Item Cost is below 400
</commit_message>
<xml_diff>
--- a/working_with_conditions.xlsx
+++ b/working_with_conditions.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HP\Desktop\Projects\Data_Analysis_Portfolio\working_with_conditions\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4984338-7221-4A06-9D16-D83D65777A10}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D98A9B81-21EC-4BD4-B55B-D4D9FB3E51B8}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7545" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="42">
   <si>
     <t>Name</t>
   </si>
@@ -143,6 +143,9 @@
   </si>
   <si>
     <t>Max sales (NY)</t>
+  </si>
+  <si>
+    <t>Max sale (NY) w/ item val &lt;$400</t>
   </si>
 </sst>
 </file>
@@ -432,8 +435,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
-      <selection activeCell="K13" sqref="K13"/>
+    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
+      <selection activeCell="J15" sqref="J15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.25" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -446,7 +449,7 @@
     <col min="6" max="6" width="16" customWidth="1"/>
     <col min="7" max="7" width="11.125" customWidth="1"/>
     <col min="8" max="8" width="8.625" customWidth="1"/>
-    <col min="9" max="9" width="15.25" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="28.625" bestFit="1" customWidth="1"/>
     <col min="10" max="24" width="10.5" customWidth="1"/>
   </cols>
   <sheetData>
@@ -828,6 +831,13 @@
       <c r="H14" s="5" t="s">
         <v>28</v>
       </c>
+      <c r="I14" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="J14">
+        <f>_xlfn.MAXIFS(D2:D21, B2:B21, "NY", E2:E21, "&lt;400")</f>
+        <v>964.69</v>
+      </c>
     </row>
     <row r="15" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">

</xml_diff>